<commit_message>
wykres kołowy i kolumnowy
</commit_message>
<xml_diff>
--- a/RankingTOPSIS.xlsx
+++ b/RankingTOPSIS.xlsx
@@ -22,52 +22,52 @@
     <t>Location</t>
   </si>
   <si>
+    <t>MAŁOPOLSKIE</t>
+  </si>
+  <si>
+    <t>POMORSKIE</t>
+  </si>
+  <si>
+    <t>DOLNOŚLĄSKIE</t>
+  </si>
+  <si>
+    <t>ŚLĄSKIE</t>
+  </si>
+  <si>
     <t>MAZOWIECKIE</t>
   </si>
   <si>
-    <t>POMORSKIE</t>
-  </si>
-  <si>
-    <t>DOLNOŚLĄSKIE</t>
-  </si>
-  <si>
-    <t>MAŁOPOLSKIE</t>
-  </si>
-  <si>
-    <t>ŚLĄSKIE</t>
+    <t>ŁÓDZKIE</t>
+  </si>
+  <si>
+    <t>ZACHODNIOPOMORSKIE</t>
+  </si>
+  <si>
+    <t>PODKARPACKIE</t>
+  </si>
+  <si>
+    <t>LUBUSKIE</t>
+  </si>
+  <si>
+    <t>LUBELSKIE</t>
+  </si>
+  <si>
+    <t>ŚWIĘTOKRZYSKIE</t>
+  </si>
+  <si>
+    <t>WARMIŃSKO-MAZURSKIE</t>
+  </si>
+  <si>
+    <t>PODLASKIE</t>
+  </si>
+  <si>
+    <t>OPOLSKIE</t>
   </si>
   <si>
     <t>WIELKOPOLSKIE</t>
   </si>
   <si>
-    <t>ŁÓDZKIE</t>
-  </si>
-  <si>
-    <t>ZACHODNIOPOMORSKIE</t>
-  </si>
-  <si>
-    <t>PODKARPACKIE</t>
-  </si>
-  <si>
-    <t>LUBUSKIE</t>
-  </si>
-  <si>
-    <t>PODLASKIE</t>
-  </si>
-  <si>
-    <t>WARMIŃSKO-MAZURSKIE</t>
-  </si>
-  <si>
-    <t>LUBELSKIE</t>
-  </si>
-  <si>
     <t>KUJAWSKO-POMORSKIE</t>
-  </si>
-  <si>
-    <t>ŚWIĘTOKRZYSKIE</t>
-  </si>
-  <si>
-    <t>OPOLSKIE</t>
   </si>
 </sst>
 </file>

</xml_diff>